<commit_message>
Modified MapChannelToProjectCode to take pos profile.
</commit_message>
<xml_diff>
--- a/Documents/Commerce7 Live-1.xlsx
+++ b/Documents/Commerce7 Live-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\client-development\bosman-commerce7-sync\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E7CE6B-28D9-4AD9-BEB0-5BC7F0E2BB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D44CD1-86FB-4D30-BE20-E65758DB45F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19395" windowHeight="21540" xr2:uid="{22E69124-FC2A-453C-9D84-9AD8F9FB9B65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{22E69124-FC2A-453C-9D84-9AD8F9FB9B65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -188,7 +188,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -205,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -224,6 +224,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -661,13 +665,13 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -683,13 +687,13 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="10" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>